<commit_message>
Updated list of technicians for dropdowns.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_capture_v4_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_capture_v4_4_0.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="111">
   <si>
     <t xml:space="preserve">Capture Preparation Template</t>
   </si>
@@ -354,7 +354,7 @@
     <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
   </si>
   <si>
-    <t xml:space="preserve">Lena Li Chun Fong</t>
+    <t xml:space="preserve">Ariane Boisclair</t>
   </si>
   <si>
     <t xml:space="preserve">MCC-Seq ImmuneV2 (ImmuneV3B)</t>
@@ -378,7 +378,7 @@
     <t xml:space="preserve">Tube Strip 3x1</t>
   </si>
   <si>
-    <t xml:space="preserve">Leïla Drissi Kaitouni</t>
+    <t xml:space="preserve">Antoine Farley</t>
   </si>
   <si>
     <t xml:space="preserve">SureSelect Human All Exon V6 + UTRs</t>
@@ -387,10 +387,13 @@
     <t xml:space="preserve">Tube Strip 4x1</t>
   </si>
   <si>
-    <t xml:space="preserve">Ariane Boisclair</t>
+    <t xml:space="preserve">Lena Li</t>
   </si>
   <si>
     <t xml:space="preserve">Tube Strip 5x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girija Daliah</t>
   </si>
   <si>
     <t xml:space="preserve">Tube Strip 6x1</t>
@@ -844,7 +847,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
@@ -8814,10 +8817,6 @@
       <formula1>Index!$A$2:$A$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E380" type="list">
-      <formula1>Index!$B$2:$B$7</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K43" type="list">
       <formula1>Index!$F$2:$F$4</formula1>
       <formula2>0</formula2>
@@ -8832,6 +8831,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I380" type="list">
       <formula1>Index!$E$2:$E$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E380" type="list">
+      <formula1>Index!$B$2:$B$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -8858,7 +8861,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.3"/>
@@ -18103,7 +18106,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.4"/>
   </cols>
@@ -19630,7 +19633,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
@@ -19810,13 +19813,15 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="0" t="s">
+        <v>107</v>
+      </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19827,7 +19832,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19838,7 +19843,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23208,16 +23213,19 @@
       <c r="G385" s="13"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B386" s="13"/>
       <c r="C386" s="13"/>
       <c r="D386" s="13"/>
       <c r="E386" s="13"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B387" s="13"/>
       <c r="C387" s="13"/>
       <c r="D387" s="13"/>
       <c r="E387" s="13"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B388" s="13"/>
       <c r="E388" s="13"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add technician to the rest of templates
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_capture_v4_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_capture_v4_4_0.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="113">
   <si>
     <t xml:space="preserve">Capture Preparation Template</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tube Strip 6x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marie-Michelle Simons</t>
   </si>
   <si>
     <t xml:space="preserve">Tube Strip 7x1</t>
@@ -850,7 +853,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
@@ -8816,34 +8819,34 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B380" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B380" type="list">
       <formula1>Index!$A$2:$A$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K43" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K43" type="list">
       <formula1>Index!$F$2:$F$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:F380" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:F380" type="list">
       <formula1>Index!$C$2:$C$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H380" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H380" type="list">
       <formula1>Index!$D$2:$D$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I380" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I380" type="list">
       <formula1>Index!$E$2:$E$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E380" type="list">
-      <formula1>Index!$B$2:$B$9</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E380" type="list">
+      <formula1>Index!$B$2:$B$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8864,7 +8867,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.3"/>
@@ -18075,22 +18078,22 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5:H480" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5:H480" type="list">
       <formula1>Index!$G$2:$G$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
       <formula1>'Capture Batch'!$A$7:$A$106</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O100" type="list">
       <formula1>Index!$H$2:$H$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -18109,7 +18112,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.4"/>
   </cols>
@@ -19617,7 +19620,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -19633,10 +19636,10 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
@@ -19833,13 +19836,15 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>110</v>
+      </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19850,7 +19855,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23850,7 +23855,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add Marie-Michelle Simons to the list of lab tech (#856)
* Add Marie-Michelle Simons to the list of lab tech

* add technician to validation list

* add technician to the rest of templates

* correct cursor position

* correct cursor locations
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_capture_v4_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_capture_v4_4_0.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="113">
   <si>
     <t xml:space="preserve">Capture Preparation Template</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tube Strip 6x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marie-Michelle Simons</t>
   </si>
   <si>
     <t xml:space="preserve">Tube Strip 7x1</t>
@@ -850,7 +853,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
@@ -8816,34 +8819,34 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B380" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B380" type="list">
       <formula1>Index!$A$2:$A$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K43" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K43" type="list">
       <formula1>Index!$F$2:$F$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:F380" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:F380" type="list">
       <formula1>Index!$C$2:$C$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H380" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H380" type="list">
       <formula1>Index!$D$2:$D$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I380" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I380" type="list">
       <formula1>Index!$E$2:$E$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E380" type="list">
-      <formula1>Index!$B$2:$B$9</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E380" type="list">
+      <formula1>Index!$B$2:$B$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8864,7 +8867,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.3"/>
@@ -18075,22 +18078,22 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5:H480" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5:H480" type="list">
       <formula1>Index!$G$2:$G$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
       <formula1>'Capture Batch'!$A$7:$A$106</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O100" type="list">
       <formula1>Index!$H$2:$H$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -18109,7 +18112,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.4"/>
   </cols>
@@ -19617,7 +19620,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -19636,7 +19639,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
@@ -19833,13 +19836,15 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>110</v>
+      </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19850,7 +19855,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23850,7 +23855,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>